<commit_message>
Updated results for BoW+TFIDF Model - Lucene, Thunderbird and Ubuntu
</commit_message>
<xml_diff>
--- a/thesis-binary-relevance/binary-relevance-meka-results.xlsx
+++ b/thesis-binary-relevance/binary-relevance-meka-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="117">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -120,6 +120,57 @@
     <t xml:space="preserve">0.904 0.796 0.839 0.899 0.959</t>
   </si>
   <si>
+    <t xml:space="preserve">Count Vectorizer + TFIDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.377 0.657 0.512 0.368 0.743</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.123 0.674 0.686 0.132 0.879</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.247 0.528 0.350 0.239 0.594</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.733 0.754 0.820 0.729 0.959</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.416 0.740 0.719 0.609 0.845</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.383 0.584 0.501 0.321 0.606</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.266 0.755 0.641 0.468 0.758</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.877 0.735 0.778 0.823 0.938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.417 0.725 0.694 0.522 0.786</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.437 0.699 0.671 0.507 0.839</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.266 0.626 0.556 0.359 0.652</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.886 0.782 0.841 0.885 0.960</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.176 0.673 0.461 0.252 0.681</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.000 0.831 0.911 0.911 0.947</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.097 0.523 0.300 0.144 0.517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.904 0.803 0.838 0.899 0.957</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.488 0.410 0.332 0.494 0.416</t>
   </si>
   <si>
@@ -168,6 +219,54 @@
     <t xml:space="preserve">0.763 0.837 0.927 0.923 0.977</t>
   </si>
   <si>
+    <t xml:space="preserve">0.477 0.397 0.338 0.494 0.416</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.613 0.602 0.076 0.077 0.677</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.320 0.250 0.214 0.421 0.263</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.786 0.856 0.755 0.584 0.978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.669 0.681 0.512 0.550 0.592</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.491 0.479 0.292 0.309 0.293</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.569 0.552 0.353 0.390 0.425</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.753 0.836 0.891 0.890 0.959</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.642 0.613 0.415 0.483 0.490</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.614 0.587 0.476 0.566 0.788</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.499 0.455 0.263 0.320 0.325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.803 0.864 0.925 0.932 0.980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.315 0.302 0.229 0.266 0.462</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.892 0.935 0.879 0.921 1.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.187 0.178 0.129 0.154 0.300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.798 0.869 0.936 0.936 0.982</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.580 0.421 0.363 0.209 0.734</t>
   </si>
   <si>
@@ -228,9 +327,6 @@
     <t xml:space="preserve">0.823 0.881 0.940 0.952 0.982</t>
   </si>
   <si>
-    <t xml:space="preserve">Count Vectorizer + TFIDF</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.582 0.424 0.349 0.209 0.748</t>
   </si>
   <si>
@@ -265,6 +361,18 @@
   </si>
   <si>
     <t xml:space="preserve">0.815 0.886 0.935 0.944 0.981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.482 0.330 0.209 0.273 0.755</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.909 0.976 1.000 0.857 0.947</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.319 0.198 0.116 0.158 0.607</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.824 0.881 0.940 0.953 0.982</t>
   </si>
 </sst>
 </file>
@@ -365,21 +473,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -500,6 +608,106 @@
       </c>
       <c r="F7" s="0" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -518,21 +726,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.7551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -563,16 +771,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -583,16 +791,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -603,16 +811,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -623,16 +831,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -643,16 +851,116 @@
         <v>7</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>47</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -673,19 +981,19 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.5918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.7857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -716,16 +1024,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -736,16 +1044,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -756,16 +1064,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>59</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -776,16 +1084,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -796,16 +1104,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -813,19 +1121,19 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -833,19 +1141,19 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,19 +1161,19 @@
         <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -873,19 +1181,19 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -893,19 +1201,19 @@
         <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>66</v>
+        <v>32</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>115</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>67</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Report: Added descriptions for Section 6.1.1
</commit_message>
<xml_diff>
--- a/thesis-binary-relevance/binary-relevance-meka-results.xlsx
+++ b/thesis-binary-relevance/binary-relevance-meka-results.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="122">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -169,6 +169,21 @@
   </si>
   <si>
     <t xml:space="preserve">0.904 0.803 0.838 0.899 0.957</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.170 0.683 0.515 0.252 0.668</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.000 0.812 0.896 0.911 0.963</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.093 0.537 0.348 0.144 0.502</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.904 0.801 0.846 0.899 0.956</t>
   </si>
   <si>
     <t xml:space="preserve">0.488 0.410 0.332 0.494 0.416</t>
@@ -473,16 +488,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.7040816326531"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.4336734693878"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2448979591837"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3520408163265"/>
@@ -708,6 +723,53 @@
       </c>
       <c r="F13" s="0" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -771,16 +833,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -791,16 +853,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -811,16 +873,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -831,16 +893,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -851,16 +913,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -871,16 +933,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -891,16 +953,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -911,16 +973,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -931,16 +993,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -951,16 +1013,16 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1024,16 +1086,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1044,16 +1106,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1064,16 +1126,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1084,16 +1146,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1104,16 +1166,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1124,16 +1186,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1144,16 +1206,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1164,16 +1226,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1184,16 +1246,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1204,16 +1266,16 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Binary Relevance for SVM and MNB, CONFIG 1-5
</commit_message>
<xml_diff>
--- a/thesis-binary-relevance/binary-relevance-meka-results.xlsx
+++ b/thesis-binary-relevance/binary-relevance-meka-results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lucene" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="195">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -171,19 +171,94 @@
     <t xml:space="preserve">0.904 0.803 0.838 0.899 0.957</t>
   </si>
   <si>
+    <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.311 0.747 0.735 0.539 0.816</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.410 0.562 0.535 0.396 0.744</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.185 0.876 0.654 0.380 0.700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.886 0.727 0.797 0.861 0.954</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.426 0.728 0.671 0.500 0.709 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.418 0.705 0.698 0.511 0.905</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.274 0.628 0.523 0.338 0.551</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.883 0.785 0.844 0.886 0.957</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.342 0.773 0.742 0.590 0.825</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.372 0.602 0.538 0.327 0.659</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.208 0.841 0.667 0.444 0.720</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.879 0.758 0.799 0.830 0.945</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.421 0.739 0.667 0.507 0.743</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.422 0.714 0.669 0.492 0.885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.270 0.644 0.521 0.345 0.594</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.883 0.792 0.836 0.883 0.959</t>
+  </si>
+  <si>
     <t xml:space="preserve">Count Vectorizer + TFIDF + ngram(1)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.170 0.683 0.515 0.252 0.668</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.000 0.812 0.896 0.911 0.963</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.093 0.537 0.348 0.144 0.502</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.904 0.801 0.846 0.899 0.956</t>
+    <t xml:space="preserve">CV + TFIDF + ngram(3) + stopwords</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.388 0.768 0.729 0.578 0.815</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.423 0.592 0.547 0.356 0.646</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.243 0.854 0.639 0.426 0.705</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.885 0.751 0.803 0.844 0.942</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.374 0.736 0.613 0.420 0.717</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.429 0.744 0.690 0.547 0.928</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.232 0.628 0.455 0.268 0.560</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.886 0.801 0.834 0.889 0.959</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CV + TFIDF + ngram(3) + stopwords + Lemm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.423 0.592 0.547 0.356 0.646 </t>
   </si>
   <si>
     <t xml:space="preserve">0.488 0.410 0.332 0.494 0.416</t>
@@ -282,6 +357,78 @@
     <t xml:space="preserve">0.798 0.869 0.936 0.936 0.982</t>
   </si>
   <si>
+    <t xml:space="preserve">0.698 0.622 0.332 0.481 0.570</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.481 0.466 0.300 0.417 0.582</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.631 0.475 0.201 0.320 0.400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.746 0.832 0.908 0.917 0.977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.622 0.598 0.409 0.425 0.447</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.588 0.555 0.397 0.463 0.958</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.477 0.440 0.259 0.272 0.288</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.793 0.857 0.918 0.923 0.981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.696 0.665 0.434 0.531 0.556</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.478 0.461 0.325 0.368 0.437</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.628 0.533 0.281 0.368 0.388</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.744 0.829 0.905 0.907 0.971</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.627 0.602 0.404 0.436 0.431</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.590 0.553 0.500 0.448 0.917</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.483 0.444 0.254 0.281 0.275</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.794 0.856 0.927 0.921 0.981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.662 0.621 0.367 0.508 0.582</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.483 0.471 0.263 0.359 0.452</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.560 0.473 0.228 0.346 0.413</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.749 0.834 0.898 0.906 0.972</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.582 0.538 0.333 0.409 0.447</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.595 0.550 0.433 0.465 0.920</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.428 0.376 0.201 0.259 0.288</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.791 0.854 0.923 0.923 0.981</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.580 0.421 0.363 0.209 0.734</t>
   </si>
   <si>
@@ -388,6 +535,78 @@
   </si>
   <si>
     <t xml:space="preserve">0.824 0.881 0.940 0.953 0.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.750 0.676 0.427 0.406 0.685</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.491 0.456 0.280 0.394 0.884</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.755 0.546 0.275 0.257 0.521</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.747 0.837 0.903 0.938 0.977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.679 0.621 0.326 0.311 0.808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.629 0.618 0.430 0.622 0.721</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.547 0.461 0.196 0.184 0.684</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.808 0.879 0.928 0.949 0.976</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.766 0.687 0.382 0.430 0.774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.506 0.446 0.352 0.344 0.860</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.783 0.563 0.238 0.276 0.632</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.758 0.832 0.918 0.932 0.980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.679 0.608 0.234 0.320 0.798</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.637 0.618 0.758 0.879 0.804</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.546 0.446 0.132 0.191 0.667</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.811 0.878 0.938 0.954 0.979</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.744 0.719 0.396 0.430 0.691</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.467 0.460 0.388 0.353 0.756</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.786 0.610 0.249 0.276 0.530</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.726 0.837 0.922 0.933 0.973</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.652 0.546 0.217 0.282 0.760</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.647 0.664 0.920 0.893 0.837 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.508 0.380 0.122 0.164 0.615</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.810 0.880 0.940 0.953 0.979</t>
   </si>
 </sst>
 </file>
@@ -488,16 +707,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.7040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.9030612244898"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.4336734693878"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2448979591837"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3520408163265"/>
@@ -725,51 +944,211 @@
         <v>48</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>53</v>
+      <c r="C16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -788,10 +1167,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -833,16 +1212,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,16 +1232,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -873,16 +1252,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -893,16 +1272,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -913,16 +1292,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -933,16 +1312,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,16 +1332,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,16 +1352,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -993,16 +1372,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1013,16 +1392,221 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>85</v>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1041,10 +1625,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1086,16 +1670,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>87</v>
+        <v>136</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>88</v>
+        <v>137</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>89</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1106,16 +1690,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>90</v>
+        <v>139</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>91</v>
+        <v>140</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>92</v>
+        <v>141</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>93</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1126,16 +1710,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>94</v>
+        <v>143</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>95</v>
+        <v>144</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>96</v>
+        <v>145</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>97</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1146,16 +1730,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>100</v>
+        <v>149</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>101</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1166,16 +1750,16 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>102</v>
+        <v>151</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>103</v>
+        <v>152</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>104</v>
+        <v>153</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>105</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1186,16 +1770,16 @@
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>106</v>
+        <v>155</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>107</v>
+        <v>156</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>109</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1206,16 +1790,16 @@
         <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>110</v>
+        <v>159</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>111</v>
+        <v>160</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>112</v>
+        <v>161</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1226,16 +1810,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>114</v>
+        <v>163</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>115</v>
+        <v>164</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>116</v>
+        <v>165</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1246,16 +1830,16 @@
         <v>32</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>100</v>
+        <v>149</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>101</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1266,16 +1850,221 @@
         <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>118</v>
+        <v>167</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>119</v>
+        <v>168</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>120</v>
+        <v>169</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>121</v>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>